<commit_message>
Basic version of morningstar_stats_class.py:  fetches the data correctly from Morningstar
</commit_message>
<xml_diff>
--- a/src/montecarlo_multi_out.xlsx
+++ b/src/montecarlo_multi_out.xlsx
@@ -3578,229 +3578,229 @@
         <v>28</v>
       </c>
       <c r="B2">
-        <v>145216862.66</v>
+        <v>112186436.73</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>5079462.59</v>
+        <v>949876.27</v>
       </c>
       <c r="E2">
-        <v>14021914.57</v>
+        <v>9049342.050000001</v>
       </c>
       <c r="F2">
-        <v>5206284.99</v>
+        <v>-273433.18</v>
       </c>
       <c r="G2">
-        <v>5280888.47</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>28717689.07</v>
+        <v>12243394.18</v>
       </c>
       <c r="I2">
-        <v>5547214.87</v>
+        <v>2646153.86</v>
       </c>
       <c r="J2">
-        <v>76324161.42</v>
+        <v>59299813.38</v>
       </c>
       <c r="K2">
-        <v>14330098.14</v>
+        <v>8140315.9</v>
       </c>
       <c r="L2">
-        <v>27733439.98</v>
+        <v>19394703.97</v>
       </c>
       <c r="M2">
-        <v>22385748.12</v>
+        <v>15751661.2</v>
       </c>
       <c r="N2">
-        <v>7401712.27</v>
+        <v>4078063.85</v>
       </c>
       <c r="O2">
-        <v>29877133.28</v>
+        <v>20078585.44</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>257670256.98</v>
+        <v>199410823.28</v>
       </c>
       <c r="R2">
-        <v>44094314.72</v>
+        <v>33394142.52</v>
       </c>
       <c r="S2">
-        <v>118484525</v>
+        <v>96152506.36</v>
       </c>
       <c r="T2">
-        <v>19692641.5</v>
+        <v>12055622.7</v>
       </c>
       <c r="U2">
-        <v>20137602.76</v>
+        <v>14067054.58</v>
       </c>
       <c r="V2">
-        <v>46133767.16</v>
+        <v>35458458.55</v>
       </c>
       <c r="W2">
-        <v>25031571.15</v>
+        <v>15062319.49</v>
       </c>
       <c r="X2">
-        <v>81435931.02</v>
+        <v>58919491.72</v>
       </c>
       <c r="Y2">
-        <v>1267596.85</v>
+        <v>-155477.56</v>
       </c>
       <c r="Z2">
-        <v>5118466.02</v>
+        <v>2941036.87</v>
       </c>
       <c r="AA2">
-        <v>9553945.449999999</v>
+        <v>5240354.25</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>40426597.82</v>
+        <v>25257955.68</v>
       </c>
       <c r="AD2">
-        <v>40870067.39</v>
+        <v>30408914.89</v>
       </c>
       <c r="AE2">
-        <v>24201745.38</v>
+        <v>17939366.72</v>
       </c>
       <c r="AF2">
-        <v>13968166.5</v>
+        <v>6009155.18</v>
       </c>
       <c r="AG2">
-        <v>9994670.380000001</v>
+        <v>6873271.76</v>
       </c>
       <c r="AH2">
-        <v>88830804.52</v>
+        <v>66746670.95</v>
       </c>
       <c r="AI2">
-        <v>40231278.87</v>
+        <v>31876486.84</v>
       </c>
       <c r="AJ2">
-        <v>288004906</v>
+        <v>228402877.46</v>
       </c>
       <c r="AK2">
-        <v>7217442.88</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>42236324.46</v>
+        <v>31432003.97</v>
       </c>
       <c r="AM2">
-        <v>31085391.34</v>
+        <v>17724790</v>
       </c>
       <c r="AN2">
         <v>0</v>
       </c>
       <c r="AO2">
-        <v>11866456.1</v>
+        <v>6459880.81</v>
       </c>
       <c r="AP2">
-        <v>1979410.99</v>
+        <v>472425.44</v>
       </c>
       <c r="AQ2">
-        <v>70940429.67</v>
+        <v>54823649.7</v>
       </c>
       <c r="AR2">
-        <v>16649688.56</v>
+        <v>10159480.5</v>
       </c>
       <c r="AS2">
-        <v>62366236.57</v>
+        <v>45480575.49</v>
       </c>
       <c r="AT2">
-        <v>14285234.39</v>
+        <v>10027318.81</v>
       </c>
       <c r="AU2">
-        <v>4435000.11</v>
+        <v>1281963.45</v>
       </c>
       <c r="AV2">
         <v>0</v>
       </c>
       <c r="AW2">
-        <v>1178181.04</v>
+        <v>-161935.12</v>
       </c>
       <c r="AX2">
-        <v>14779303.49</v>
+        <v>10902861.83</v>
       </c>
       <c r="AY2">
-        <v>6169472.74</v>
+        <v>1195942.67</v>
       </c>
       <c r="AZ2">
-        <v>75155083.33</v>
+        <v>59851334.36</v>
       </c>
       <c r="BA2">
-        <v>8253393.41</v>
+        <v>3620250.88</v>
       </c>
       <c r="BB2">
-        <v>40750849.01</v>
+        <v>30782005.6</v>
       </c>
       <c r="BC2">
-        <v>81283497.98999999</v>
+        <v>62052071.28</v>
       </c>
       <c r="BD2">
-        <v>268265.87</v>
+        <v>-350217.95</v>
       </c>
       <c r="BE2">
-        <v>129793245.03</v>
+        <v>98348347.98999999</v>
       </c>
       <c r="BF2">
         <v>0</v>
       </c>
       <c r="BG2">
-        <v>4313858.84</v>
+        <v>2272433.25</v>
       </c>
       <c r="BH2">
-        <v>625101600.66</v>
+        <v>516989963.38</v>
       </c>
       <c r="BI2">
         <v>0</v>
       </c>
       <c r="BJ2">
-        <v>84123732.08</v>
+        <v>61306732.85</v>
       </c>
       <c r="BK2">
-        <v>11774673.33</v>
+        <v>8646051.92</v>
       </c>
       <c r="BL2">
-        <v>79786372.73</v>
+        <v>58907525.44</v>
       </c>
       <c r="BM2">
-        <v>126615701.76</v>
+        <v>102624872.94</v>
       </c>
       <c r="BN2">
-        <v>19495202.14</v>
+        <v>14432633.82</v>
       </c>
       <c r="BO2">
-        <v>10689099.18</v>
+        <v>7337269.6</v>
       </c>
       <c r="BP2">
-        <v>18201769.19</v>
+        <v>11793094.31</v>
       </c>
       <c r="BQ2">
-        <v>1886219.23</v>
+        <v>235247.08</v>
       </c>
       <c r="BR2">
-        <v>132188529.97</v>
+        <v>107563381.61</v>
       </c>
       <c r="BS2">
-        <v>6743662.94</v>
+        <v>3673430.39</v>
       </c>
       <c r="BT2">
-        <v>144558836.96</v>
+        <v>112656242.18</v>
       </c>
       <c r="BU2">
         <v>0</v>
       </c>
       <c r="BV2">
-        <v>44095561.8</v>
+        <v>23690234.13</v>
       </c>
       <c r="BW2">
-        <v>18442083.04</v>
+        <v>10785328.76</v>
       </c>
       <c r="BX2">
-        <v>117338442.23</v>
+        <v>78521210.66</v>
       </c>
       <c r="BY2">
         <v>0</v>
@@ -3809,25 +3809,25 @@
         <v>0</v>
       </c>
       <c r="CA2">
-        <v>22387068.42</v>
+        <v>15522899.32</v>
       </c>
       <c r="CB2">
-        <v>5346935.01</v>
+        <v>0</v>
       </c>
       <c r="CC2">
-        <v>2461447.19</v>
+        <v>0</v>
       </c>
       <c r="CD2">
-        <v>47580856.07</v>
+        <v>36759931.57</v>
       </c>
       <c r="CE2">
-        <v>16208088.41</v>
+        <v>10372366.58</v>
       </c>
       <c r="CF2">
-        <v>70219645.14</v>
+        <v>50757641.24</v>
       </c>
       <c r="CG2">
-        <v>6093224.62</v>
+        <v>2195049.46</v>
       </c>
       <c r="CH2">
         <v>0</v>
@@ -3836,46 +3836,46 @@
         <v>0</v>
       </c>
       <c r="CJ2">
-        <v>202715381.18</v>
+        <v>166766207.22</v>
       </c>
       <c r="CK2">
-        <v>43142459.09</v>
+        <v>32974031.03</v>
       </c>
       <c r="CL2">
-        <v>19884425.64</v>
+        <v>12583245.94</v>
       </c>
       <c r="CM2">
-        <v>4874611.5</v>
+        <v>2471782.27</v>
       </c>
       <c r="CN2">
-        <v>35228569.49</v>
+        <v>25451101.36</v>
       </c>
       <c r="CO2">
-        <v>27415380.75</v>
+        <v>18793746.08</v>
       </c>
       <c r="CP2">
-        <v>77133340.45999999</v>
+        <v>61075352.18</v>
       </c>
       <c r="CQ2">
-        <v>8204629.9</v>
+        <v>4873958.19</v>
       </c>
       <c r="CR2">
-        <v>15223604.4</v>
+        <v>10784133.13</v>
       </c>
       <c r="CS2">
-        <v>46765844.91</v>
+        <v>34619060.22</v>
       </c>
       <c r="CT2">
-        <v>264276258.93</v>
+        <v>214352530.27</v>
       </c>
       <c r="CU2">
-        <v>8067645.67</v>
+        <v>4590835.49</v>
       </c>
       <c r="CV2">
-        <v>1038500.81</v>
+        <v>-120114.76</v>
       </c>
       <c r="CW2">
-        <v>15017451.41</v>
+        <v>10444527.3</v>
       </c>
     </row>
     <row r="3" spans="1:101">
@@ -3883,22 +3883,22 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>10254.76</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>697076.5</v>
+        <v>-25148.61</v>
       </c>
       <c r="D3">
-        <v>988802.45</v>
+        <v>437018.85</v>
       </c>
       <c r="E3">
-        <v>188183.3</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>325330.64</v>
+        <v>76109.34</v>
       </c>
       <c r="G3">
-        <v>354068.63</v>
+        <v>-357020.79</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3907,10 +3907,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>128700.65</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>73234.42999999999</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -3919,268 +3919,268 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>674794.58</v>
+        <v>258232.23</v>
       </c>
       <c r="O3">
-        <v>83250.81</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>-238171.86</v>
+        <v>-778.11</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>395670.12</v>
+        <v>71987.83</v>
       </c>
       <c r="S3">
-        <v>479812.59</v>
+        <v>104886.84</v>
       </c>
       <c r="T3">
-        <v>143620.98</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>138031.37</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1166157.97</v>
+        <v>659659.23</v>
       </c>
       <c r="W3">
-        <v>1076961.6</v>
+        <v>545860.3199999999</v>
       </c>
       <c r="X3">
-        <v>1768784.39</v>
+        <v>1223019.43</v>
       </c>
       <c r="Y3">
-        <v>255883.43</v>
+        <v>140874.33</v>
       </c>
       <c r="Z3">
-        <v>680753.73</v>
+        <v>269024.24</v>
       </c>
       <c r="AA3">
-        <v>728964.08</v>
+        <v>241593.45</v>
       </c>
       <c r="AB3">
-        <v>-353.78</v>
+        <v>-25534.63</v>
       </c>
       <c r="AC3">
-        <v>1257157.56</v>
+        <v>836263.5600000001</v>
       </c>
       <c r="AD3">
-        <v>924376.38</v>
+        <v>457064.27</v>
       </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3">
-        <v>1255219.15</v>
+        <v>732086.1800000001</v>
       </c>
       <c r="AG3">
-        <v>493355.21</v>
+        <v>167352.85</v>
       </c>
       <c r="AH3">
         <v>0</v>
       </c>
       <c r="AI3">
-        <v>715093.9399999999</v>
+        <v>352497.87</v>
       </c>
       <c r="AJ3">
-        <v>553465.5600000001</v>
+        <v>141506.21</v>
       </c>
       <c r="AK3">
-        <v>921842.96</v>
+        <v>-16451.3</v>
       </c>
       <c r="AL3">
-        <v>522898.76</v>
+        <v>156438.46</v>
       </c>
       <c r="AM3">
-        <v>423059.6</v>
+        <v>122986.8</v>
       </c>
       <c r="AN3">
-        <v>-144152.11</v>
+        <v>-91369.7</v>
       </c>
       <c r="AO3">
-        <v>283800.41</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>343080.65</v>
+        <v>74434.60000000001</v>
       </c>
       <c r="AQ3">
-        <v>297178.85</v>
+        <v>19402.44</v>
       </c>
       <c r="AR3">
-        <v>744968.86</v>
+        <v>395686.59</v>
       </c>
       <c r="AS3">
         <v>0</v>
       </c>
       <c r="AT3">
-        <v>707251.6800000001</v>
+        <v>299026.82</v>
       </c>
       <c r="AU3">
-        <v>35851.82</v>
+        <v>0</v>
       </c>
       <c r="AV3">
-        <v>-4673.02</v>
+        <v>-57927.76</v>
       </c>
       <c r="AW3">
-        <v>347163.48</v>
+        <v>33192.07</v>
       </c>
       <c r="AX3">
-        <v>534005.64</v>
+        <v>202866.61</v>
       </c>
       <c r="AY3">
-        <v>318287.28</v>
+        <v>43725.19</v>
       </c>
       <c r="AZ3">
-        <v>843007.9</v>
+        <v>488256.3</v>
       </c>
       <c r="BA3">
-        <v>355816.78</v>
+        <v>0</v>
       </c>
       <c r="BB3">
-        <v>1061436.34</v>
+        <v>655927.73</v>
       </c>
       <c r="BC3">
-        <v>634992.61</v>
+        <v>235643.65</v>
       </c>
       <c r="BD3">
-        <v>425302.83</v>
+        <v>215285.88</v>
       </c>
       <c r="BE3">
         <v>0</v>
       </c>
       <c r="BF3">
-        <v>-47565.02</v>
+        <v>-5146.65</v>
       </c>
       <c r="BG3">
-        <v>148930.47</v>
+        <v>0</v>
       </c>
       <c r="BH3">
-        <v>1571402.38</v>
+        <v>869853.0600000001</v>
       </c>
       <c r="BI3">
-        <v>7548.49</v>
+        <v>18088.14</v>
       </c>
       <c r="BJ3">
-        <v>511496.79</v>
+        <v>211571.96</v>
       </c>
       <c r="BK3">
-        <v>854995.9300000001</v>
+        <v>419671.38</v>
       </c>
       <c r="BL3">
         <v>0</v>
       </c>
       <c r="BM3">
-        <v>182425.31</v>
+        <v>0</v>
       </c>
       <c r="BN3">
-        <v>1194472.24</v>
+        <v>591690.14</v>
       </c>
       <c r="BO3">
-        <v>388039.02</v>
+        <v>78435.10000000001</v>
       </c>
       <c r="BP3">
-        <v>411379.45</v>
+        <v>89068.63</v>
       </c>
       <c r="BQ3">
         <v>0</v>
       </c>
       <c r="BR3">
-        <v>1256116.95</v>
+        <v>767001.02</v>
       </c>
       <c r="BS3">
         <v>0</v>
       </c>
       <c r="BT3">
-        <v>953085.4</v>
+        <v>583882.85</v>
       </c>
       <c r="BU3">
-        <v>-244425.67</v>
+        <v>-83860.10000000001</v>
       </c>
       <c r="BV3">
-        <v>404250.94</v>
+        <v>52739.96</v>
       </c>
       <c r="BW3">
-        <v>385648.2</v>
+        <v>82880.78999999999</v>
       </c>
       <c r="BX3">
-        <v>385642.86</v>
+        <v>54160.26</v>
       </c>
       <c r="BY3">
-        <v>-62149.01</v>
+        <v>-137207.23</v>
       </c>
       <c r="BZ3">
-        <v>-85810.91</v>
+        <v>-226583.76</v>
       </c>
       <c r="CA3">
-        <v>589692.51</v>
+        <v>253643.67</v>
       </c>
       <c r="CB3">
-        <v>804348.4</v>
+        <v>-1667.35</v>
       </c>
       <c r="CC3">
-        <v>792159.54</v>
+        <v>355324.13</v>
       </c>
       <c r="CD3">
-        <v>146356.95</v>
+        <v>0</v>
       </c>
       <c r="CE3">
-        <v>238321.25</v>
+        <v>0</v>
       </c>
       <c r="CF3">
-        <v>119433.94</v>
+        <v>0</v>
       </c>
       <c r="CG3">
-        <v>565408.4300000001</v>
+        <v>244312.17</v>
       </c>
       <c r="CH3">
-        <v>-99478.61</v>
+        <v>-128070.79</v>
       </c>
       <c r="CI3">
-        <v>-116146.47</v>
+        <v>-124743.69</v>
       </c>
       <c r="CJ3">
-        <v>840447.13</v>
+        <v>380608.53</v>
       </c>
       <c r="CK3">
-        <v>1673551.09</v>
+        <v>1123450.63</v>
       </c>
       <c r="CL3">
-        <v>238780.26</v>
+        <v>0</v>
       </c>
       <c r="CM3">
-        <v>390949.57</v>
+        <v>48790.99</v>
       </c>
       <c r="CN3">
-        <v>1183506.86</v>
+        <v>687033.67</v>
       </c>
       <c r="CO3">
-        <v>588397.9</v>
+        <v>258414.87</v>
       </c>
       <c r="CP3">
-        <v>214667.09</v>
+        <v>0</v>
       </c>
       <c r="CQ3">
-        <v>142211.31</v>
+        <v>0</v>
       </c>
       <c r="CR3">
-        <v>797278.25</v>
+        <v>456527.35</v>
       </c>
       <c r="CS3">
-        <v>753193.59</v>
+        <v>307667.13</v>
       </c>
       <c r="CT3">
         <v>0</v>
       </c>
       <c r="CU3">
-        <v>655054.01</v>
+        <v>213558.1</v>
       </c>
       <c r="CV3">
         <v>0</v>
       </c>
       <c r="CW3">
-        <v>83059.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:101">
@@ -4194,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>39252.65</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -4266,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>-13835.38</v>
+        <v>-40967.78</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>38944.36</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <v>0</v>
@@ -4332,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="AX4">
-        <v>3993.77</v>
+        <v>0</v>
       </c>
       <c r="AY4">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="BI4">
-        <v>-66843.92</v>
+        <v>-23644.44</v>
       </c>
       <c r="BJ4">
         <v>0</v>
@@ -4407,7 +4407,7 @@
         <v>0</v>
       </c>
       <c r="BW4">
-        <v>10065.17</v>
+        <v>0</v>
       </c>
       <c r="BX4">
         <v>0</v>
@@ -4798,304 +4798,304 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>145227117.43</v>
+        <v>112186436.73</v>
       </c>
       <c r="C6">
-        <v>697076.5</v>
+        <v>-25148.61</v>
       </c>
       <c r="D6">
-        <v>6107517.69</v>
+        <v>1386895.11</v>
       </c>
       <c r="E6">
-        <v>14210097.86</v>
+        <v>9049342.050000001</v>
       </c>
       <c r="F6">
-        <v>5531615.63</v>
+        <v>-197323.84</v>
       </c>
       <c r="G6">
-        <v>5634957.1</v>
+        <v>-357020.79</v>
       </c>
       <c r="H6">
-        <v>28717689.07</v>
+        <v>12243394.18</v>
       </c>
       <c r="I6">
-        <v>5547214.87</v>
+        <v>2646153.86</v>
       </c>
       <c r="J6">
-        <v>76452862.06999999</v>
+        <v>59299813.38</v>
       </c>
       <c r="K6">
-        <v>14403332.56</v>
+        <v>8140315.9</v>
       </c>
       <c r="L6">
-        <v>27733439.98</v>
+        <v>19394703.97</v>
       </c>
       <c r="M6">
-        <v>22385748.12</v>
+        <v>15751661.2</v>
       </c>
       <c r="N6">
-        <v>8076506.85</v>
+        <v>4336296.08</v>
       </c>
       <c r="O6">
-        <v>29960384.09</v>
+        <v>20078585.44</v>
       </c>
       <c r="P6">
-        <v>-238171.86</v>
+        <v>-778.11</v>
       </c>
       <c r="Q6">
-        <v>257670256.98</v>
+        <v>199410823.28</v>
       </c>
       <c r="R6">
-        <v>44489984.85</v>
+        <v>33466130.35</v>
       </c>
       <c r="S6">
-        <v>118964337.59</v>
+        <v>96257393.20999999</v>
       </c>
       <c r="T6">
-        <v>19836262.49</v>
+        <v>12055622.7</v>
       </c>
       <c r="U6">
-        <v>20275634.13</v>
+        <v>14067054.58</v>
       </c>
       <c r="V6">
-        <v>47299925.13</v>
+        <v>36118117.78</v>
       </c>
       <c r="W6">
-        <v>26108532.75</v>
+        <v>15608179.81</v>
       </c>
       <c r="X6">
-        <v>83204715.41</v>
+        <v>60142511.15</v>
       </c>
       <c r="Y6">
-        <v>1523480.28</v>
+        <v>-14603.24</v>
       </c>
       <c r="Z6">
-        <v>5799219.76</v>
+        <v>3210061.11</v>
       </c>
       <c r="AA6">
-        <v>10282909.53</v>
+        <v>5481947.7</v>
       </c>
       <c r="AB6">
-        <v>-14189.16</v>
+        <v>-66502.39999999999</v>
       </c>
       <c r="AC6">
-        <v>41683755.38</v>
+        <v>26094219.23</v>
       </c>
       <c r="AD6">
-        <v>41794443.76</v>
+        <v>30865979.16</v>
       </c>
       <c r="AE6">
-        <v>24201745.38</v>
+        <v>17939366.72</v>
       </c>
       <c r="AF6">
-        <v>15223385.65</v>
+        <v>6741241.36</v>
       </c>
       <c r="AG6">
-        <v>10488025.59</v>
+        <v>7040624.62</v>
       </c>
       <c r="AH6">
-        <v>88869748.88</v>
+        <v>66746670.95</v>
       </c>
       <c r="AI6">
-        <v>40946372.81</v>
+        <v>32228984.71</v>
       </c>
       <c r="AJ6">
-        <v>288558371.57</v>
+        <v>228544383.68</v>
       </c>
       <c r="AK6">
-        <v>8139285.84</v>
+        <v>-16451.3</v>
       </c>
       <c r="AL6">
-        <v>42759223.23</v>
+        <v>31588442.43</v>
       </c>
       <c r="AM6">
-        <v>31508450.94</v>
+        <v>17847776.8</v>
       </c>
       <c r="AN6">
-        <v>-144152.11</v>
+        <v>-91369.7</v>
       </c>
       <c r="AO6">
-        <v>12150256.5</v>
+        <v>6459880.81</v>
       </c>
       <c r="AP6">
-        <v>2322491.64</v>
+        <v>546860.03</v>
       </c>
       <c r="AQ6">
-        <v>71237608.52</v>
+        <v>54843052.13</v>
       </c>
       <c r="AR6">
-        <v>17394657.42</v>
+        <v>10555167.1</v>
       </c>
       <c r="AS6">
-        <v>62366236.57</v>
+        <v>45480575.49</v>
       </c>
       <c r="AT6">
-        <v>14992486.06</v>
+        <v>10326345.63</v>
       </c>
       <c r="AU6">
-        <v>4470851.93</v>
+        <v>1281963.45</v>
       </c>
       <c r="AV6">
-        <v>-4673.02</v>
+        <v>-57927.76</v>
       </c>
       <c r="AW6">
-        <v>1525344.52</v>
+        <v>-128743.05</v>
       </c>
       <c r="AX6">
-        <v>15317302.9</v>
+        <v>11105728.43</v>
       </c>
       <c r="AY6">
-        <v>6487760.02</v>
+        <v>1239667.86</v>
       </c>
       <c r="AZ6">
-        <v>75998091.22</v>
+        <v>60339590.66</v>
       </c>
       <c r="BA6">
-        <v>8609210.199999999</v>
+        <v>3620250.88</v>
       </c>
       <c r="BB6">
-        <v>41812285.35</v>
+        <v>31437933.33</v>
       </c>
       <c r="BC6">
-        <v>81918490.59999999</v>
+        <v>62287714.93</v>
       </c>
       <c r="BD6">
-        <v>693568.7</v>
+        <v>-134932.07</v>
       </c>
       <c r="BE6">
-        <v>129793245.03</v>
+        <v>98348347.98999999</v>
       </c>
       <c r="BF6">
-        <v>-47565.02</v>
+        <v>-5146.65</v>
       </c>
       <c r="BG6">
-        <v>4462789.31</v>
+        <v>2272433.25</v>
       </c>
       <c r="BH6">
-        <v>626673003.04</v>
+        <v>517859816.43</v>
       </c>
       <c r="BI6">
-        <v>-59295.44</v>
+        <v>-5556.3</v>
       </c>
       <c r="BJ6">
-        <v>84635228.87</v>
+        <v>61518304.81</v>
       </c>
       <c r="BK6">
-        <v>12629669.26</v>
+        <v>9065723.300000001</v>
       </c>
       <c r="BL6">
-        <v>79786372.73</v>
+        <v>58907525.44</v>
       </c>
       <c r="BM6">
-        <v>126798127.07</v>
+        <v>102624872.94</v>
       </c>
       <c r="BN6">
-        <v>20689674.38</v>
+        <v>15024323.96</v>
       </c>
       <c r="BO6">
-        <v>11077138.19</v>
+        <v>7415704.7</v>
       </c>
       <c r="BP6">
-        <v>18613148.64</v>
+        <v>11882162.94</v>
       </c>
       <c r="BQ6">
-        <v>1886219.23</v>
+        <v>235247.08</v>
       </c>
       <c r="BR6">
-        <v>133444646.92</v>
+        <v>108330382.63</v>
       </c>
       <c r="BS6">
-        <v>6743662.94</v>
+        <v>3673430.39</v>
       </c>
       <c r="BT6">
-        <v>145511922.36</v>
+        <v>113240125.03</v>
       </c>
       <c r="BU6">
-        <v>-244425.67</v>
+        <v>-83860.10000000001</v>
       </c>
       <c r="BV6">
-        <v>44499812.74</v>
+        <v>23742974.1</v>
       </c>
       <c r="BW6">
-        <v>18837796.41</v>
+        <v>10868209.55</v>
       </c>
       <c r="BX6">
-        <v>117724085.09</v>
+        <v>78575370.92</v>
       </c>
       <c r="BY6">
-        <v>-62149.01</v>
+        <v>-137207.23</v>
       </c>
       <c r="BZ6">
-        <v>-85810.91</v>
+        <v>-226583.76</v>
       </c>
       <c r="CA6">
-        <v>22976760.93</v>
+        <v>15776542.99</v>
       </c>
       <c r="CB6">
-        <v>6151283.41</v>
+        <v>-1667.35</v>
       </c>
       <c r="CC6">
-        <v>3253606.73</v>
+        <v>355324.13</v>
       </c>
       <c r="CD6">
-        <v>47727213.02</v>
+        <v>36759931.57</v>
       </c>
       <c r="CE6">
-        <v>16446409.66</v>
+        <v>10372366.58</v>
       </c>
       <c r="CF6">
-        <v>70339079.08</v>
+        <v>50757641.24</v>
       </c>
       <c r="CG6">
-        <v>6658633.05</v>
+        <v>2439361.63</v>
       </c>
       <c r="CH6">
-        <v>-99478.61</v>
+        <v>-128070.79</v>
       </c>
       <c r="CI6">
-        <v>-116146.47</v>
+        <v>-124743.69</v>
       </c>
       <c r="CJ6">
-        <v>203555828.31</v>
+        <v>167146815.75</v>
       </c>
       <c r="CK6">
-        <v>44816010.18</v>
+        <v>34097481.66</v>
       </c>
       <c r="CL6">
-        <v>20123205.91</v>
+        <v>12583245.94</v>
       </c>
       <c r="CM6">
-        <v>5265561.07</v>
+        <v>2520573.26</v>
       </c>
       <c r="CN6">
-        <v>36412076.35</v>
+        <v>26138135.03</v>
       </c>
       <c r="CO6">
-        <v>28003778.65</v>
+        <v>19052160.95</v>
       </c>
       <c r="CP6">
-        <v>77348007.55</v>
+        <v>61075352.18</v>
       </c>
       <c r="CQ6">
-        <v>8346841.21</v>
+        <v>4873958.19</v>
       </c>
       <c r="CR6">
-        <v>16020882.64</v>
+        <v>11240660.48</v>
       </c>
       <c r="CS6">
-        <v>47519038.5</v>
+        <v>34926727.35</v>
       </c>
       <c r="CT6">
-        <v>264276258.93</v>
+        <v>214352530.27</v>
       </c>
       <c r="CU6">
-        <v>8722699.68</v>
+        <v>4804393.59</v>
       </c>
       <c r="CV6">
-        <v>1038500.81</v>
+        <v>-120114.76</v>
       </c>
       <c r="CW6">
-        <v>15100510.86</v>
+        <v>10444527.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>